<commit_message>
Stub in all activities Fix always-disco scripts to use all plugins
</commit_message>
<xml_diff>
--- a/docs/TODO-Oct-16.xlsx
+++ b/docs/TODO-Oct-16.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="0" windowWidth="19440" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="700" yWindow="0" windowWidth="22840" windowHeight="18620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="88">
   <si>
     <t>Task</t>
   </si>
@@ -226,9 +226,6 @@
   </si>
   <si>
     <t>Health Tips</t>
-  </si>
-  <si>
-    <t>Neu:Zessie</t>
   </si>
   <si>
     <t>Scripts</t>
@@ -802,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -820,7 +817,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1">
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
@@ -1055,7 +1052,7 @@
         <v>34</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1">
@@ -1075,7 +1072,7 @@
         <v>65</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1">
@@ -1086,7 +1083,7 @@
     <row r="21" spans="1:7" ht="18" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="7">
         <v>2</v>
@@ -1101,7 +1098,7 @@
         <v>34</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1">
@@ -1121,7 +1118,7 @@
         <v>34</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1">
@@ -1141,7 +1138,7 @@
         <v>34</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1">
@@ -1161,7 +1158,7 @@
         <v>34</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1">
@@ -1175,13 +1172,13 @@
         <v>4</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1">
@@ -1281,7 +1278,7 @@
         <v>48</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>62</v>
@@ -1298,7 +1295,7 @@
         <v>47</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>56</v>
@@ -1315,13 +1312,13 @@
         <v>20</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1">
@@ -1335,7 +1332,7 @@
         <v>46</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>35</v>
@@ -1355,7 +1352,7 @@
         <v>48</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>50</v>
@@ -1372,10 +1369,10 @@
         <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>53</v>
@@ -1406,7 +1403,7 @@
         <v>64</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1">
@@ -1527,7 +1524,7 @@
     </row>
     <row r="49" spans="1:6" ht="18" customHeight="1">
       <c r="B49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="7">
         <f>SUMIF(E9:E39,"=NEU:Writer",C9:C39)</f>
@@ -1540,7 +1537,7 @@
     </row>
     <row r="50" spans="1:6" ht="18" customHeight="1">
       <c r="B50" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="7">
         <f>SUM(C36)</f>
@@ -1563,10 +1560,10 @@
     </row>
     <row r="53" spans="1:6" ht="18" customHeight="1">
       <c r="A53" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" customHeight="1">
@@ -1574,166 +1571,166 @@
         <v>55</v>
       </c>
       <c r="C54" s="7">
-        <f>C43*8</f>
+        <f t="shared" ref="C54:D61" si="0">C43*8</f>
         <v>120</v>
       </c>
       <c r="D54" s="7">
-        <f>D43*8</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="E54" s="1">
-        <f>C43/2</f>
+        <f t="shared" ref="E54:F61" si="1">C43/2</f>
         <v>7.5</v>
       </c>
       <c r="F54" s="1">
-        <f>D43/2</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" customHeight="1">
       <c r="B55" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C55" s="7">
-        <f>C44*8</f>
+        <f t="shared" si="0"/>
         <v>168</v>
       </c>
       <c r="D55" s="7">
-        <f>D44*8</f>
+        <f t="shared" si="0"/>
         <v>248</v>
       </c>
       <c r="E55" s="1">
-        <f>C44/2</f>
+        <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
       <c r="F55" s="1">
-        <f>D44/2</f>
+        <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" customHeight="1">
       <c r="B56" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="7">
-        <f>C45*8</f>
+        <f t="shared" si="0"/>
         <v>152</v>
       </c>
       <c r="D56" s="7">
-        <f>D45*8</f>
+        <f t="shared" si="0"/>
         <v>272</v>
       </c>
       <c r="E56" s="1">
-        <f>C45/2</f>
+        <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
       <c r="F56" s="1">
-        <f>D45/2</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" customHeight="1">
       <c r="B57" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="7">
-        <f>C46*8</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="D57" s="7">
-        <f>D46*8</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="E57" s="1">
-        <f>C46/2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F57" s="1">
-        <f>D46/2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" customHeight="1">
       <c r="B58" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C58" s="7">
-        <f>C47*8</f>
+        <f t="shared" si="0"/>
         <v>232</v>
       </c>
       <c r="D58" s="7">
-        <f>D47*8</f>
+        <f t="shared" si="0"/>
         <v>472</v>
       </c>
       <c r="E58" s="1">
-        <f>C47/2</f>
+        <f t="shared" si="1"/>
         <v>14.5</v>
       </c>
       <c r="F58" s="1">
-        <f>D47/2</f>
+        <f t="shared" si="1"/>
         <v>29.5</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="18" customHeight="1">
       <c r="B59" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="7">
-        <f>C48*8</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="D59" s="7">
-        <f>D48*8</f>
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="E59" s="1">
-        <f>C48/2</f>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
       <c r="F59" s="1">
-        <f>D48/2</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="18" customHeight="1">
       <c r="B60" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="7">
-        <f>C49*8</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="D60" s="7">
-        <f>D49*8</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="E60" s="1">
-        <f>C49/2</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="F60" s="1">
-        <f>D49/2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="18" customHeight="1">
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C61" s="7">
-        <f>C50*8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D61" s="7">
-        <f>D50*8</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="E61" s="1">
-        <f>C50/2</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="F61" s="1">
-        <f>D50/2</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>

</xml_diff>